<commit_message>
Adding the Get bill function
</commit_message>
<xml_diff>
--- a/bills/app/in/rates.xlsx
+++ b/bills/app/in/rates.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t xml:space="preserve">Product</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t xml:space="preserve">Valencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product2</t>
   </si>
 </sst>
 </file>
@@ -70,6 +79,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -140,12 +150,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -155,10 +165,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -309,13 +319,57 @@
         <v>45</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>